<commit_message>
adding benthic and invert code
</commit_message>
<xml_diff>
--- a/reef monitoring/data/npa_ltm.xlsx
+++ b/reef monitoring/data/npa_ltm.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/npa/reef monitoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3C98F9-B766-1747-9948-14BB8604E3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA8C3E-EAAF-5E47-89D8-10FF158FBA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="460" windowWidth="17860" windowHeight="16040" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
+    <workbookView xWindow="7720" yWindow="460" windowWidth="17860" windowHeight="16040" activeTab="1" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
-    <sheet name="benthic_algae" sheetId="2" r:id="rId2"/>
-    <sheet name="benthic_inverts" sheetId="3" r:id="rId3"/>
+    <sheet name="benthic" sheetId="2" r:id="rId2"/>
+    <sheet name="inverts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
   <si>
     <t>Surveyor</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Turf algal height</t>
   </si>
   <si>
-    <t>Macroalgae height</t>
-  </si>
-  <si>
     <t>MWW</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>Snapper</t>
+  </si>
+  <si>
+    <t>Conch</t>
+  </si>
+  <si>
+    <t>Macroalgal height</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E07F57-2AAC-D84A-ABDD-038A618CED61}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -637,10 +640,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -655,19 +658,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>28</v>
       </c>
       <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -675,10 +678,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <v>44842</v>
@@ -693,19 +696,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -713,10 +716,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2">
         <v>44842</v>
@@ -731,19 +734,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -751,10 +754,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <v>44842</v>
@@ -769,19 +772,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -792,10 +795,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>44842</v>
@@ -810,19 +813,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="M6">
         <v>7</v>
@@ -830,10 +833,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
         <v>44842</v>
@@ -848,19 +851,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -868,10 +871,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2">
         <v>44477</v>
@@ -886,19 +889,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8">
         <v>28</v>
       </c>
       <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
         <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -906,10 +909,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>44477</v>
@@ -924,19 +927,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9">
         <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -944,10 +947,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <v>44477</v>
@@ -962,19 +965,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10">
         <v>28</v>
       </c>
       <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" t="s">
         <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>23</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -982,10 +985,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2">
         <v>44477</v>
@@ -1000,19 +1003,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11">
         <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M11">
         <v>2</v>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3343D824-2265-BC42-99AD-C0B9372F937A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1075,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>17</v>
@@ -1080,10 +1083,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -1098,13 +1101,13 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1140,10 +1143,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D6BD88-263F-1D48-A268-1DAE3FDA2569}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1170,10 +1173,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -1182,10 +1185,110 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding benthic and invert graphs
</commit_message>
<xml_diff>
--- a/reef monitoring/data/npa_ltm.xlsx
+++ b/reef monitoring/data/npa_ltm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/npa/reef monitoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA8C3E-EAAF-5E47-89D8-10FF158FBA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6014CD59-A1EF-CE45-8532-305A85951CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="460" windowWidth="17860" windowHeight="16040" activeTab="1" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
+    <workbookView xWindow="880" yWindow="680" windowWidth="17860" windowHeight="16040" activeTab="2" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
   <si>
     <t>Surveyor</t>
   </si>
@@ -137,16 +137,13 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Invertebrate type</t>
-  </si>
-  <si>
     <t>Side</t>
   </si>
   <si>
     <t>Meter</t>
   </si>
   <si>
-    <t>Turf algal height</t>
+    <t>Macroalgae height</t>
   </si>
   <si>
     <t>MWW</t>
@@ -191,7 +188,7 @@
     <t>Conch</t>
   </si>
   <si>
-    <t>Macroalgal height</t>
+    <t>Turf height</t>
   </si>
 </sst>
 </file>
@@ -640,10 +637,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -658,19 +655,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>28</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="M2">
         <v>5</v>
@@ -678,10 +675,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>44842</v>
@@ -696,19 +693,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -716,10 +713,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <v>44842</v>
@@ -734,19 +731,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -754,10 +751,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>44842</v>
@@ -772,19 +769,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -795,10 +792,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>44842</v>
@@ -813,19 +810,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="M6">
         <v>7</v>
@@ -833,10 +830,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>44842</v>
@@ -851,19 +848,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -871,10 +868,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>44477</v>
@@ -889,19 +886,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>28</v>
       </c>
       <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
         <v>21</v>
-      </c>
-      <c r="K8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" t="s">
-        <v>22</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -909,10 +906,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <v>44477</v>
@@ -927,19 +924,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9">
         <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -947,10 +944,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
         <v>44477</v>
@@ -965,19 +962,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10">
         <v>28</v>
       </c>
       <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
         <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" t="s">
-        <v>22</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -985,10 +982,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2">
         <v>44477</v>
@@ -1003,19 +1000,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11">
         <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M11">
         <v>2</v>
@@ -1029,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3343D824-2265-BC42-99AD-C0B9372F937A}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,24 +1066,24 @@
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -1101,13 +1098,13 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1123,6 +1120,33 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>10.1</v>
+      </c>
+      <c r="F3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
       <c r="K3">
         <v>1</v>
       </c>
@@ -1134,6 +1158,88 @@
       </c>
       <c r="N3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>10.1</v>
+      </c>
+      <c r="F4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10.1</v>
+      </c>
+      <c r="F5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1145,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D6BD88-263F-1D48-A268-1DAE3FDA2569}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1165,7 +1271,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -1173,10 +1279,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -1185,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1193,10 +1299,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>44842</v>
@@ -1205,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1213,10 +1319,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <v>44842</v>
@@ -1225,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1233,10 +1339,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>44477</v>
@@ -1245,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1253,10 +1359,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>44477</v>
@@ -1265,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1273,10 +1379,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>44477</v>
@@ -1285,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>3</v>

</xml_diff>

<commit_message>
new fish graphs for NPA monitoring
</commit_message>
<xml_diff>
--- a/reef monitoring/data/npa_ltm.xlsx
+++ b/reef monitoring/data/npa_ltm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/npa/reef monitoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBBB0EA-4309-7545-A06A-525C5A8BA095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEDD244-ED9B-9548-A6C9-496E1BB05E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="680" windowWidth="17860" windowHeight="16040" activeTab="2" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
+    <workbookView xWindow="880" yWindow="680" windowWidth="17860" windowHeight="16040" activeTab="1" xr2:uid="{94001EFB-2903-7B43-8B82-BDDB464EFE6D}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
   <si>
     <t>Surveyor</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>Size over 70cm</t>
+  </si>
+  <si>
+    <t>Diadema</t>
+  </si>
+  <si>
+    <t>Mermaids</t>
+  </si>
+  <si>
+    <t>Pillars</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3343D824-2265-BC42-99AD-C0B9372F937A}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,6 +1251,170 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>10.1</v>
+      </c>
+      <c r="F6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>10.1</v>
+      </c>
+      <c r="F7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>10.1</v>
+      </c>
+      <c r="F8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>10.1</v>
+      </c>
+      <c r="F9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1249,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D6BD88-263F-1D48-A268-1DAE3FDA2569}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,7 +1455,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2">
         <v>44842</v>
@@ -1302,7 +1475,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>44842</v>
@@ -1322,13 +1495,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2">
         <v>44842</v>
       </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -1342,7 +1515,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2">
         <v>44477</v>
@@ -1362,7 +1535,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2">
         <v>44477</v>
@@ -1382,7 +1555,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2">
         <v>44477</v>
@@ -1395,6 +1568,206 @@
       </c>
       <c r="F7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44842</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44477</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>